<commit_message>
update robot with bakery sample for CI/CD
</commit_message>
<xml_diff>
--- a/src/test/resources/data/in/loginLogout.xlsx
+++ b/src/test/resources/data/in/loginLogout.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>user</t>
   </si>
@@ -25,16 +25,22 @@
     <t>Result</t>
   </si>
   <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>password1</t>
-  </si>
-  <si>
-    <t>user2</t>
-  </si>
-  <si>
-    <t>password2</t>
+    <t>℗:qmTAYKS9UG87rNuUQ0Ao6Q==</t>
+  </si>
+  <si>
+    <t>sgrillon</t>
+  </si>
+  <si>
+    <t>sgrillon2</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>referencer</t>
   </si>
 </sst>
 </file>
@@ -401,42 +407,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>